<commit_message>
update excel method summary
</commit_message>
<xml_diff>
--- a/crypto_method_assignments.xlsx
+++ b/crypto_method_assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_jasthi\_Teacher_Master_D0_NOT_DELETE_TWO\_CS421_Python\SILC\cryptoquote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC861AB-060C-4FE2-AC8D-EE47146E91C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46D79F7-D9EA-46C3-8220-67A7782B6EE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="117">
   <si>
     <t>Aare</t>
   </si>
@@ -335,6 +335,42 @@
   </si>
   <si>
     <t>getAuthorAndQuoteCount( )</t>
+  </si>
+  <si>
+    <t>Waiting Pull Request</t>
+  </si>
+  <si>
+    <t>Pull Request is in</t>
+  </si>
+  <si>
+    <t>Jasthi</t>
+  </si>
+  <si>
+    <t>Siva</t>
+  </si>
+  <si>
+    <t>Return the list of Quotes which contains some swear words</t>
+  </si>
+  <si>
+    <t>def getQuotesContainingBadWords()</t>
+  </si>
+  <si>
+    <t>def showRandomCryptoInHTML( )</t>
+  </si>
+  <si>
+    <t>def updateQuote(id,quote, author,submitted_by)</t>
+  </si>
+  <si>
+    <t>def getRandomQuote( )</t>
+  </si>
+  <si>
+    <t>def deleteQuote(id)</t>
+  </si>
+  <si>
+    <t>def addQuote(quote, author,submitted_by)</t>
+  </si>
+  <si>
+    <t>def getStudentWithLeastQuotes()</t>
   </si>
 </sst>
 </file>
@@ -839,7 +875,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -849,6 +885,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1204,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,10 +1255,11 @@
     <col min="4" max="4" width="83.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="32.88671875" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.77734375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="21.88671875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
@@ -1240,8 +1278,11 @@
       <c r="F1" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="5">
+        <v>44268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1255,7 +1296,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1269,7 +1310,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1289,7 +1330,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1305,8 +1346,11 @@
       <c r="E5" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1322,8 +1366,11 @@
       <c r="E6" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1343,7 +1390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1359,8 +1406,11 @@
       <c r="E8" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1373,11 +1423,14 @@
       <c r="D9" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1390,8 +1443,11 @@
       <c r="D10" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1405,7 +1461,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1425,7 +1481,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1441,8 +1497,11 @@
       <c r="E13" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1462,7 +1521,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1479,7 +1538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1492,8 +1551,11 @@
       <c r="D16" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1513,7 +1575,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1533,7 +1595,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1546,8 +1608,11 @@
       <c r="D19" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1567,7 +1632,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1587,7 +1652,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1607,7 +1672,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1627,7 +1692,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1647,7 +1712,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1666,8 +1731,11 @@
       <c r="F25" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1680,8 +1748,14 @@
       <c r="D26" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1701,7 +1775,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1714,8 +1788,14 @@
       <c r="D28" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1727,6 +1807,32 @@
       </c>
       <c r="D29" s="2" t="s">
         <v>61</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to crypto (with comments and structure)
</commit_message>
<xml_diff>
--- a/crypto_method_assignments.xlsx
+++ b/crypto_method_assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_jasthi\_Teacher_Master_D0_NOT_DELETE_TWO\_CS421_Python\SILC\cryptoquote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42CEC9F-D126-4202-AF02-67D044D216CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AE6D47-4AFB-4EA3-97E8-EFAC33D00EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
   <si>
     <t>Aare</t>
   </si>
@@ -395,6 +395,15 @@
   </si>
   <si>
     <t>Delete a quote from the collection</t>
+  </si>
+  <si>
+    <t>def getQuotesContainingGoodWords()</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Return the list of Quotes which contains some good words</t>
   </si>
 </sst>
 </file>
@@ -1265,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,6 +1929,26 @@
         <v>121</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
     <sortCondition ref="B2:B29"/>

</xml_diff>

<commit_message>
Updates crypto.py and assignment status
</commit_message>
<xml_diff>
--- a/crypto_method_assignments.xlsx
+++ b/crypto_method_assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_jasthi\_Teacher_Master_D0_NOT_DELETE_TWO\_CS421_Python\SILC\cryptoquote\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AE6D47-4AFB-4EA3-97E8-EFAC33D00EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11805DE4-F3F9-4BEE-8269-670BD4653BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
   <si>
     <t>Aare</t>
   </si>
@@ -404,6 +404,12 @@
   </si>
   <si>
     <t>Return the list of Quotes which contains some good words</t>
+  </si>
+  <si>
+    <t>Somasekhar Motukuri</t>
+  </si>
+  <si>
+    <t>Nikhita Gollamudi</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,6 +735,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF87AFC6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,7 +944,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -919,6 +955,26 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1274,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,14 +1341,15 @@
     <col min="1" max="1" width="3.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="10.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="83.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
@@ -1302,20 +1359,21 @@
       <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="5">
+      <c r="H1" s="5">
         <v>44268</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1325,71 +1383,78 @@
       <c r="C2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="G4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1399,37 +1464,39 @@
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1439,497 +1506,526 @@
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="G9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="G11" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="G12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="G15" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="13"/>
+      <c r="E17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="G17" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="G18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="G20" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="G21" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="G22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="G23" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="G24" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="G25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="G26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="G27" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3"/>
+      <c r="E28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="G28" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="G29" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+      <c r="G30" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="G31" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1939,18 +2035,18 @@
       <c r="C33" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
     <sortCondition ref="B2:B29"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>